<commit_message>
add sample for manual QA gen from excel
</commit_message>
<xml_diff>
--- a/tools/manual_qa_gen/template.xlsx
+++ b/tools/manual_qa_gen/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiba\work\github\dasadc\gen_adc_qa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiba\work\github\dasadc\adc2019\tools\manual_qa_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A62E22-94C6-41C7-B486-0BB033DE8074}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ED6FCA-2BE7-4235-BA29-0C4E77668F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9024" activeTab="2" xr2:uid="{4544EA2B-CE45-4D74-A9A2-5E4E3CCD59A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4544EA2B-CE45-4D74-A9A2-5E4E3CCD59A9}"/>
   </bookViews>
   <sheets>
     <sheet name="lines" sheetId="1" r:id="rId1"/>
@@ -100,6 +100,699 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="吹き出し: 四角形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{058367E6-0259-4ACA-B819-AE0ECA78931C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5425440" y="304800"/>
+          <a:ext cx="3055620" cy="2918460"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -60484"/>
+            <a:gd name="adj2" fmla="val 15227"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>このシートでは解答例となる</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
+            <a:t>配線を記入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>します。</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
+            <a:t>配線番号を各マスに記入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>してください。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>また、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
+            <a:t>ブロック位置に相当し、かつ配線のない箇所については </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+            <a:t>"+" </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
+            <a:t>を記入</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ください。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>このシートはＱ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>Ａの生成のため必須です。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>※</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>色分けは不要です。見やすさのためにここでは適当に色づけしています。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>※</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>この吹き出しは消しても構いません。無視されます。</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="吹き出し: 四角形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BCBB656-E89A-4243-A176-C60DCEF66358}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5074920" y="228600"/>
+          <a:ext cx="3055620" cy="3802380"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -60484"/>
+            <a:gd name="adj2" fmla="val 15227"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>このシートでは各ブロック（番号付き）の位置を指定します。</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ブロックを包含する矩形の左上に相当する一にのみ、ブロックの番号を記入してください。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>このシートはＱ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Ａの生成のため必須です。</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ＡだけでなくＱも生成したい場合、このブロック番号は、 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>blocks </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>シートでのブロック番号と整合している必要があります</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+          </a:br>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>※</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>色分けは不要です。見やすさのためにここでは適当に色づけしています。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>※</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>この吹き出しは消しても構いません。無視されます。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="吹き出し: 四角形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{752A7DBA-A671-4029-A56B-F1C813BF2A78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5448300" y="167640"/>
+          <a:ext cx="3055620" cy="3749040"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -60484"/>
+            <a:gd name="adj2" fmla="val 15227"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>このシートでは各ブロックに番号を割り当てます。</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Q</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の生成用で、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>A</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>を生成するだけなら不要です。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
+            <a:t>同じブロックのマスをすべて同じ番号で埋めてください。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>この番号は、 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>blockpos </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>シートで指定した番号と整合している必要があります</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>このシートはＱの生成のため必須です。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>の生成だけでよい場合、不要です。</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>※</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>色分けは不要です。見やすさのためにここでは適当に色づけしています。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>※</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>この吹き出しは消しても構いません。無視されます。</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465A2BA0-FEF8-4934-B341-4E0B4D85D8A8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.69921875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -413,6 +1106,7 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -421,7 +1115,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.69921875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -431,6 +1125,7 @@
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -438,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9E5B4E-11BC-4C04-AA69-ADE6E5DEC049}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -449,5 +1144,6 @@
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>